<commit_message>
Add test for kohdentumattomat paatokset
</commit_message>
<xml_diff>
--- a/tests/data/test_viranomaispaatokset/paatokset.xlsx
+++ b/tests/data/test_viranomaispaatokset/paatokset.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="63">
   <si>
     <t xml:space="preserve">Otsikko</t>
   </si>
@@ -182,20 +182,52 @@
   </si>
   <si>
     <t xml:space="preserve">1.7.2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">119/2022 Otsikko</t>
+  </si>
+  <si>
+    <t xml:space="preserve">119/2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vastaanottaja Nurmi Paavo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">987654321Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keskeyttäminen myönteinen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Paavo Nurmen tie 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00250</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Helsinki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">118/2022 Otsikko</t>
+  </si>
+  <si>
+    <t xml:space="preserve">118/2022</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -219,6 +251,11 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -262,25 +299,37 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -300,275 +349,368 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R5"/>
+  <dimension ref="A1:R7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L7" activeCellId="0" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="22.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="29.76"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="17.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="45.76"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="17.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="17.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="22.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="22.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="29.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="17.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="45.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="17.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="17.38"/>
   </cols>
   <sheetData>
-    <row r="1" s="2" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+    <row r="1" s="3" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="E2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="F2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G2" s="0" t="s">
+      <c r="G2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="H2" s="0" t="s">
+      <c r="H2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="J2" s="0" t="s">
+      <c r="J2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="K2" s="0" t="s">
+      <c r="K2" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="L2" s="0" t="s">
+      <c r="L2" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="M2" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="N2" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="O2" s="0" t="n">
+      <c r="O2" s="1" t="n">
         <v>15100</v>
       </c>
-      <c r="P2" s="0" t="s">
+      <c r="P2" s="1" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="F3" s="0" t="s">
+      <c r="F3" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="G3" s="0" t="s">
+      <c r="G3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H3" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="I3" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="J3" s="0" t="s">
+      <c r="J3" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="K3" s="0" t="s">
+      <c r="K3" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="L3" s="0" t="s">
+      <c r="L3" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="M3" s="4" t="n">
+      <c r="M3" s="5" t="n">
         <v>26</v>
       </c>
-      <c r="N3" s="3" t="s">
+      <c r="N3" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="O3" s="3" t="n">
+      <c r="O3" s="4" t="n">
         <v>15100</v>
       </c>
-      <c r="P3" s="3" t="s">
+      <c r="P3" s="4" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D4" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="F4" s="0" t="s">
+      <c r="F4" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="G4" s="0" t="s">
+      <c r="G4" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="I4" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="J4" s="0" t="s">
+      <c r="J4" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="K4" s="0" t="s">
+      <c r="K4" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="L4" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="M4" s="4" t="s">
+      <c r="M4" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="N4" s="0" t="s">
+      <c r="N4" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="O4" s="0" t="n">
+      <c r="O4" s="1" t="n">
         <v>16200</v>
       </c>
-      <c r="P4" s="0" t="s">
+      <c r="P4" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="D5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="F5" s="0" t="s">
+      <c r="F5" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="G5" s="0" t="s">
+      <c r="G5" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="H5" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="I5" s="3" t="s">
+      <c r="I5" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="J5" s="0" t="s">
+      <c r="J5" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="K5" s="0" t="s">
+      <c r="K5" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="L5" s="3" t="s">
+      <c r="L5" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="M5" s="4"/>
-      <c r="N5" s="3" t="s">
+      <c r="M5" s="5"/>
+      <c r="N5" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="O5" s="3" t="n">
+      <c r="O5" s="4" t="n">
         <v>16200</v>
       </c>
-      <c r="P5" s="3" t="s">
+      <c r="P5" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="K6" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="L6" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="O6" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="P6" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="L7" s="4"/>
+      <c r="M7" s="5"/>
+      <c r="N7" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="O7" s="4" t="n">
+        <v>16200</v>
+      </c>
+      <c r="P7" s="4" t="s">
         <v>47</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add more invalid values for invalid paatos in test data
</commit_message>
<xml_diff>
--- a/tests/data/test_viranomaispaatokset/paatokset.xlsx
+++ b/tests/data/test_viranomaispaatokset/paatokset.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="65">
   <si>
     <t xml:space="preserve">Otsikko</t>
   </si>
@@ -212,6 +212,12 @@
   </si>
   <si>
     <t xml:space="preserve">118/2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tyhjennysväli ok</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pidennetty</t>
   </si>
 </sst>
 </file>
@@ -222,7 +228,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -251,11 +257,6 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -299,7 +300,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -322,10 +323,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -351,8 +348,8 @@
   </sheetPr>
   <dimension ref="A1:R7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L7" activeCellId="0" sqref="L7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J8" activeCellId="0" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -628,16 +625,16 @@
       <c r="B6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="D6" s="1" t="s">
         <v>21</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="F6" s="0" t="s">
+      <c r="F6" s="1" t="s">
         <v>54</v>
       </c>
       <c r="G6" s="1" t="s">
@@ -646,25 +643,25 @@
       <c r="H6" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="I6" s="6" t="s">
+      <c r="I6" s="4" t="s">
         <v>56</v>
       </c>
       <c r="J6" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="K6" s="0" t="s">
+      <c r="K6" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="L6" s="0" t="s">
+      <c r="L6" s="1" t="s">
         <v>38</v>
       </c>
       <c r="N6" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="O6" s="7" t="s">
+      <c r="O6" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="P6" s="0" t="s">
+      <c r="P6" s="1" t="s">
         <v>60</v>
       </c>
     </row>
@@ -687,9 +684,6 @@
       <c r="F7" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="G7" s="1" t="s">
-        <v>50</v>
-      </c>
       <c r="H7" s="4" t="s">
         <v>25</v>
       </c>
@@ -697,13 +691,15 @@
         <v>42</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="K7" s="1" t="s">
         <v>52</v>
       </c>
       <c r="L7" s="4"/>
-      <c r="M7" s="5"/>
+      <c r="M7" s="5" t="s">
+        <v>64</v>
+      </c>
       <c r="N7" s="4" t="s">
         <v>46</v>
       </c>

</xml_diff>

<commit_message>
Add check for tapahtumalaji validity for paatokset, also test case
</commit_message>
<xml_diff>
--- a/tests/data/test_viranomaispaatokset/paatokset.xlsx
+++ b/tests/data/test_viranomaispaatokset/paatokset.xlsx
@@ -214,7 +214,7 @@
     <t xml:space="preserve">118/2022</t>
   </si>
   <si>
-    <t xml:space="preserve">Tyhjennysväli ok</t>
+    <t xml:space="preserve">Tyhjennys ok</t>
   </si>
   <si>
     <t xml:space="preserve">pidennetty</t>
@@ -348,7 +348,7 @@
   </sheetPr>
   <dimension ref="A1:R7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="J8" activeCellId="0" sqref="J8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add validating start and end dates for paatos
</commit_message>
<xml_diff>
--- a/tests/data/test_viranomaispaatokset/paatokset.xlsx
+++ b/tests/data/test_viranomaispaatokset/paatokset.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="66">
   <si>
     <t xml:space="preserve">Otsikko</t>
   </si>
@@ -215,6 +215,9 @@
   </si>
   <si>
     <t xml:space="preserve">Tyhjennys ok</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.6.2022</t>
   </si>
   <si>
     <t xml:space="preserve">pidennetty</t>
@@ -349,7 +352,7 @@
   <dimension ref="A1:R7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J8" activeCellId="0" sqref="J8"/>
+      <selection pane="topLeft" activeCell="L8" activeCellId="0" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -696,9 +699,11 @@
       <c r="K7" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="L7" s="4"/>
+      <c r="L7" s="4" t="s">
+        <v>64</v>
+      </c>
       <c r="M7" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="N7" s="4" t="s">
         <v>46</v>

</xml_diff>

<commit_message>
Make address optional for paatokset
</commit_message>
<xml_diff>
--- a/tests/data/test_viranomaispaatokset/paatokset.xlsx
+++ b/tests/data/test_viranomaispaatokset/paatokset.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="66">
   <si>
     <t xml:space="preserve">Otsikko</t>
   </si>
@@ -352,7 +352,7 @@
   <dimension ref="A1:R7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L8" activeCellId="0" sqref="L8"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -513,15 +513,9 @@
       <c r="M3" s="5" t="n">
         <v>26</v>
       </c>
-      <c r="N3" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="O3" s="4" t="n">
-        <v>15100</v>
-      </c>
-      <c r="P3" s="4" t="s">
-        <v>32</v>
-      </c>
+      <c r="N3" s="4"/>
+      <c r="O3" s="4"/>
+      <c r="P3" s="4"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">

</xml_diff>

<commit_message>
Add test for negative decision of tyhjennysvali
</commit_message>
<xml_diff>
--- a/tests/data/test_viranomaispaatokset/paatokset.xlsx
+++ b/tests/data/test_viranomaispaatokset/paatokset.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="71">
   <si>
     <t xml:space="preserve">Otsikko</t>
   </si>
@@ -221,6 +221,21 @@
   </si>
   <si>
     <t xml:space="preserve">pidennetty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">117/2022 Otsikko</t>
+  </si>
+  <si>
+    <t xml:space="preserve">117/2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tyhjennysväli kielteinen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.1.2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.10.2023</t>
   </si>
 </sst>
 </file>
@@ -349,10 +364,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R7"/>
+  <dimension ref="A1:R8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -709,6 +724,48 @@
         <v>47</v>
       </c>
     </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="M8" s="5"/>
+      <c r="N8" s="4"/>
+      <c r="O8" s="4"/>
+      <c r="P8" s="4"/>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Make tapahtumalaji and paatostulos case insensitive
</commit_message>
<xml_diff>
--- a/tests/data/test_viranomaispaatokset/paatokset.xlsx
+++ b/tests/data/test_viranomaispaatokset/paatokset.xlsx
@@ -106,7 +106,7 @@
     <t xml:space="preserve">123456789A</t>
   </si>
   <si>
-    <t xml:space="preserve">AKP myönteinen</t>
+    <t xml:space="preserve">AKP Myönteinen</t>
   </si>
   <si>
     <t xml:space="preserve">1.1.2020</t>
@@ -178,7 +178,7 @@
     <t xml:space="preserve">vastaanottaja Mikkolainen Matti</t>
   </si>
   <si>
-    <t xml:space="preserve">Keskeyttäminen kielteinen</t>
+    <t xml:space="preserve">Keskeyttäminen Kielteinen</t>
   </si>
   <si>
     <t xml:space="preserve">1.7.2022</t>
@@ -367,7 +367,7 @@
   <dimension ref="A1:R8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="topLeft" activeCell="J6" activeCellId="0" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>